<commit_message>
added antrag and updatet Arbeitsstunden.xlsx
</commit_message>
<xml_diff>
--- a/syp/Arbeitsstunden.xlsx
+++ b/syp/Arbeitsstunden.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\paul\HTL_Leonding\3.Klasse\WMC\JMPSpriteWebsite\syp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC92BC05-0C2A-4D0D-90B0-81B30CFB5596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9099A9D1-61A4-4BE8-8E0C-D20314B02EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
   <si>
     <t>Jannis Katsanis</t>
   </si>
@@ -63,9 +63,6 @@
     <t>3h</t>
   </si>
   <si>
-    <t>Erste Mockup Version</t>
-  </si>
-  <si>
     <t>Projektauftrag finalisiert</t>
   </si>
   <si>
@@ -75,7 +72,16 @@
     <t>Projekt speichern angefangen</t>
   </si>
   <si>
-    <t>4h</t>
+    <t>Pflichtenheft weiter geschrieben</t>
+  </si>
+  <si>
+    <t>Mockups gemacht</t>
+  </si>
+  <si>
+    <t>Issue Number</t>
+  </si>
+  <si>
+    <t>Organisatorische Sachen geupdatet</t>
   </si>
 </sst>
 </file>
@@ -91,7 +97,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,6 +116,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -123,11 +135,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -408,37 +421,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.77734375" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="9" max="9" width="24.77734375" customWidth="1"/>
+    <col min="11" max="11" width="30.33203125" customWidth="1"/>
+    <col min="14" max="14" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="2"/>
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="K1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -448,114 +465,150 @@
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E4" t="s">
+      <c r="N3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4" s="3">
         <v>45364</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="3">
+        <v>45357</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="3">
+        <v>45371</v>
+      </c>
+      <c r="K5" t="s">
         <v>12</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="3">
+        <v>45364</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="3">
+        <v>45385</v>
+      </c>
+      <c r="K6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="3">
+        <v>45364</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="3">
+        <v>45392</v>
+      </c>
+      <c r="K7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7" s="3">
+        <v>45385</v>
+      </c>
+      <c r="N7">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="3">
-        <v>45357</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="3">
-        <v>45371</v>
-      </c>
-      <c r="I5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" t="s">
-        <v>7</v>
-      </c>
-      <c r="K5" s="3">
-        <v>45364</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="H8" s="3">
+        <v>45399</v>
+      </c>
+      <c r="K8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="3">
-        <v>45385</v>
-      </c>
-      <c r="I6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" s="3">
-        <v>45385</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="3">
-        <v>45392</v>
-      </c>
-      <c r="I7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K7" s="3">
+      <c r="M8" s="3">
         <v>45399</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="3">
-        <v>45399</v>
+      <c r="N8">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" s="3">
+        <v>45406</v>
       </c>
     </row>
   </sheetData>

</xml_diff>